<commit_message>
Copy pasted code. Now goes through both A AND B. But holy moley is this more annoying than I thought. Renaming A's to B's and B's to A's is fudgey. Going to turn it into a func
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -10,6 +10,8 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="A" sheetId="1" state="visible" r:id="rId1"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="B" sheetId="2" state="visible" r:id="rId2"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="A Sorted" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="A Sorted1" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="B Sorted" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1" refMode="A1" iterate="0" iterateCount="100" iterateDelta="0.0001"/>
@@ -899,6 +901,235 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
+      <c r="A1" s="3" t="inlineStr">
+        <is>
+          <t>AAAA</t>
+        </is>
+      </c>
+      <c r="B1" s="3" t="inlineStr">
+        <is>
+          <t>A col B</t>
+        </is>
+      </c>
+      <c r="C1" s="3" t="n">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="3" t="inlineStr">
+        <is>
+          <t>AAAA</t>
+        </is>
+      </c>
+      <c r="B3" s="3" t="inlineStr">
+        <is>
+          <t>A col B</t>
+        </is>
+      </c>
+      <c r="C3" s="3" t="n">
+        <v>998</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="inlineStr">
+        <is>
+          <t>AAAA</t>
+        </is>
+      </c>
+      <c r="B5" s="3" t="inlineStr">
+        <is>
+          <t>A col B</t>
+        </is>
+      </c>
+      <c r="C5" s="3" t="n">
+        <v>997</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="3" t="inlineStr">
+        <is>
+          <t>AAAA</t>
+        </is>
+      </c>
+      <c r="B7" s="3" t="inlineStr">
+        <is>
+          <t>A col B</t>
+        </is>
+      </c>
+      <c r="C7" s="3" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="3" t="inlineStr">
+        <is>
+          <t>BBBBB</t>
+        </is>
+      </c>
+      <c r="B8" s="3" t="inlineStr">
+        <is>
+          <t>BcolB</t>
+        </is>
+      </c>
+      <c r="C8" s="3" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="3" t="inlineStr">
+        <is>
+          <t>AAAA</t>
+        </is>
+      </c>
+      <c r="B10" s="3" t="inlineStr">
+        <is>
+          <t>A col B</t>
+        </is>
+      </c>
+      <c r="C10" s="3" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="3" t="inlineStr">
+        <is>
+          <t>BBBBB</t>
+        </is>
+      </c>
+      <c r="B11" s="3" t="inlineStr">
+        <is>
+          <t>BcolB</t>
+        </is>
+      </c>
+      <c r="C11" s="3" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="3" t="inlineStr">
+        <is>
+          <t>AAAA</t>
+        </is>
+      </c>
+      <c r="B13" s="3" t="inlineStr">
+        <is>
+          <t>A col B</t>
+        </is>
+      </c>
+      <c r="C13" s="3" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="3" t="inlineStr">
+        <is>
+          <t>BBBBB</t>
+        </is>
+      </c>
+      <c r="B14" s="3" t="inlineStr">
+        <is>
+          <t>BcolB</t>
+        </is>
+      </c>
+      <c r="C14" s="3" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="3" t="inlineStr">
+        <is>
+          <t>AAAA</t>
+        </is>
+      </c>
+      <c r="B16" s="3" t="inlineStr">
+        <is>
+          <t>A col B</t>
+        </is>
+      </c>
+      <c r="C16" s="3" t="n">
+        <v>888</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="3" t="inlineStr">
+        <is>
+          <t>AAAA</t>
+        </is>
+      </c>
+      <c r="B18" s="3" t="inlineStr">
+        <is>
+          <t>A col B</t>
+        </is>
+      </c>
+      <c r="C18" s="3" t="n">
+        <v>887</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="3" t="inlineStr">
+        <is>
+          <t>AAAA</t>
+        </is>
+      </c>
+      <c r="B20" s="3" t="inlineStr">
+        <is>
+          <t>A col B</t>
+        </is>
+      </c>
+      <c r="C20" s="3" t="n">
+        <v>886</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="3" t="inlineStr">
+        <is>
+          <t>AAAA</t>
+        </is>
+      </c>
+      <c r="B22" s="3" t="inlineStr">
+        <is>
+          <t>A col B</t>
+        </is>
+      </c>
+      <c r="C22" s="3" t="n">
+        <v>885</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="3" t="inlineStr">
+        <is>
+          <t>AAAA</t>
+        </is>
+      </c>
+      <c r="B24" s="3" t="inlineStr">
+        <is>
+          <t>A col B</t>
+        </is>
+      </c>
+      <c r="C24" s="3" t="n">
+        <v>884</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
       <c r="A1" t="inlineStr">
         <is>
           <t>AAAA</t>
@@ -1106,6 +1337,355 @@
       </c>
       <c r="C24" t="n">
         <v>884</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C40"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>BBBBB</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>BcolB</t>
+        </is>
+      </c>
+      <c r="C1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>BBBBB</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>BcolB</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>BBBBB</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>BcolB</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>BBBBB</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>BcolB</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>BBBBB</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>BcolB</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>BBBBB</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>BcolB</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>BBBBB</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>BcolB</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>BBBBB</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>BcolB</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>BBBBB</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>BcolB</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>BBBBB</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>BcolB</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>AAAA</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>A col B</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>BBBBB</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>BcolB</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>AAAA</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>A col B</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>BBBBB</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>BcolB</t>
+        </is>
+      </c>
+      <c r="C25" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>AAAA</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>A col B</t>
+        </is>
+      </c>
+      <c r="C26" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>BBBBB</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>BcolB</t>
+        </is>
+      </c>
+      <c r="C28" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>BBBBB</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>BcolB</t>
+        </is>
+      </c>
+      <c r="C30" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>BBBBB</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>BcolB</t>
+        </is>
+      </c>
+      <c r="C32" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>BBBBB</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>BcolB</t>
+        </is>
+      </c>
+      <c r="C34" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>BBBBB</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>BcolB</t>
+        </is>
+      </c>
+      <c r="C36" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>BBBBB</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>BcolB</t>
+        </is>
+      </c>
+      <c r="C38" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>BBBBB</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>BcolB</t>
+        </is>
+      </c>
+      <c r="C40" t="n">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Matcher.py for quick terminal execution. Directly saved from JN
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="A" sheetId="1" state="visible" r:id="rId1"/>
@@ -389,17 +389,18 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="13.8" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
     <col width="8.529999999999999" customWidth="1" style="3" min="1" max="1"/>
     <col width="10.57" customWidth="1" style="4" min="2" max="2"/>
-    <col width="8.529999999999999" customWidth="1" style="3" min="3" max="1025"/>
+    <col width="8.529999999999999" customWidth="1" style="4" min="3" max="3"/>
+    <col width="8.529999999999999" customWidth="1" style="3" min="4" max="1025"/>
   </cols>
   <sheetData>
     <row r="1" ht="15" customHeight="1" s="5">
@@ -413,7 +414,10 @@
           <t>A col B</t>
         </is>
       </c>
-      <c r="C1" s="3" t="n">
+      <c r="C1" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="D1" s="3" t="n">
         <v>999</v>
       </c>
     </row>
@@ -428,7 +432,10 @@
           <t>A col B</t>
         </is>
       </c>
-      <c r="C2" s="3" t="n">
+      <c r="C2" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="D2" s="3" t="n">
         <v>998</v>
       </c>
     </row>
@@ -443,7 +450,10 @@
           <t>A col B</t>
         </is>
       </c>
-      <c r="C3" s="3" t="n">
+      <c r="C3" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="D3" s="3" t="n">
         <v>997</v>
       </c>
     </row>
@@ -458,7 +468,10 @@
           <t>A col B</t>
         </is>
       </c>
-      <c r="C4" s="3" t="n">
+      <c r="C4" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="D4" s="3" t="n">
         <v>10</v>
       </c>
     </row>
@@ -473,7 +486,10 @@
           <t>A col B</t>
         </is>
       </c>
-      <c r="C5" s="3" t="n">
+      <c r="C5" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="D5" s="3" t="n">
         <v>11</v>
       </c>
     </row>
@@ -488,7 +504,10 @@
           <t>A col B</t>
         </is>
       </c>
-      <c r="C6" s="3" t="n">
+      <c r="C6" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="D6" s="3" t="n">
         <v>12</v>
       </c>
     </row>
@@ -503,7 +522,10 @@
           <t>A col B</t>
         </is>
       </c>
-      <c r="C7" s="3" t="n">
+      <c r="C7" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="D7" s="3" t="n">
         <v>888</v>
       </c>
     </row>
@@ -518,7 +540,10 @@
           <t>A col B</t>
         </is>
       </c>
-      <c r="C8" s="3" t="n">
+      <c r="C8" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="D8" s="3" t="n">
         <v>887</v>
       </c>
     </row>
@@ -533,7 +558,10 @@
           <t>A col B</t>
         </is>
       </c>
-      <c r="C9" s="3" t="n">
+      <c r="C9" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="D9" s="3" t="n">
         <v>886</v>
       </c>
     </row>
@@ -548,7 +576,10 @@
           <t>A col B</t>
         </is>
       </c>
-      <c r="C10" s="3" t="n">
+      <c r="C10" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="D10" s="3" t="n">
         <v>885</v>
       </c>
     </row>
@@ -563,7 +594,10 @@
           <t>A col B</t>
         </is>
       </c>
-      <c r="C11" s="3" t="n">
+      <c r="C11" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="D11" s="3" t="n">
         <v>884</v>
       </c>
     </row>
@@ -582,7 +616,7 @@
   </sheetPr>
   <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -891,7 +925,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -911,6 +945,9 @@
         </is>
       </c>
       <c r="C1" t="n">
+        <v>10</v>
+      </c>
+      <c r="D1" t="n">
         <v>999</v>
       </c>
     </row>
@@ -926,6 +963,9 @@
         </is>
       </c>
       <c r="C3" t="n">
+        <v>10</v>
+      </c>
+      <c r="D3" t="n">
         <v>998</v>
       </c>
     </row>
@@ -941,6 +981,9 @@
         </is>
       </c>
       <c r="C5" t="n">
+        <v>10</v>
+      </c>
+      <c r="D5" t="n">
         <v>997</v>
       </c>
     </row>
@@ -958,6 +1001,9 @@
       <c r="C7" t="n">
         <v>10</v>
       </c>
+      <c r="D7" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -986,6 +1032,9 @@
         </is>
       </c>
       <c r="C10" t="n">
+        <v>10</v>
+      </c>
+      <c r="D10" t="n">
         <v>11</v>
       </c>
     </row>
@@ -1016,6 +1065,9 @@
         </is>
       </c>
       <c r="C13" t="n">
+        <v>10</v>
+      </c>
+      <c r="D13" t="n">
         <v>12</v>
       </c>
     </row>
@@ -1046,6 +1098,9 @@
         </is>
       </c>
       <c r="C16" t="n">
+        <v>10</v>
+      </c>
+      <c r="D16" t="n">
         <v>888</v>
       </c>
     </row>
@@ -1061,6 +1116,9 @@
         </is>
       </c>
       <c r="C18" t="n">
+        <v>10</v>
+      </c>
+      <c r="D18" t="n">
         <v>887</v>
       </c>
     </row>
@@ -1076,6 +1134,9 @@
         </is>
       </c>
       <c r="C20" t="n">
+        <v>10</v>
+      </c>
+      <c r="D20" t="n">
         <v>886</v>
       </c>
     </row>
@@ -1091,6 +1152,9 @@
         </is>
       </c>
       <c r="C22" t="n">
+        <v>10</v>
+      </c>
+      <c r="D22" t="n">
         <v>885</v>
       </c>
     </row>
@@ -1106,6 +1170,9 @@
         </is>
       </c>
       <c r="C24" t="n">
+        <v>10</v>
+      </c>
+      <c r="D24" t="n">
         <v>884</v>
       </c>
     </row>
@@ -1120,7 +1187,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C40"/>
+  <dimension ref="A1:D40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1292,6 +1359,9 @@
       <c r="C20" t="n">
         <v>10</v>
       </c>
+      <c r="D20" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1320,6 +1390,9 @@
         </is>
       </c>
       <c r="C23" t="n">
+        <v>10</v>
+      </c>
+      <c r="D23" t="n">
         <v>11</v>
       </c>
     </row>
@@ -1350,6 +1423,9 @@
         </is>
       </c>
       <c r="C26" t="n">
+        <v>10</v>
+      </c>
+      <c r="D26" t="n">
         <v>12</v>
       </c>
     </row>

</xml_diff>